<commit_message>
Event Storming de notificacion y MER
</commit_message>
<xml_diff>
--- a/SpaOnline/EventStorming/Inventario Event Storming.xlsx
+++ b/SpaOnline/EventStorming/Inventario Event Storming.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grchia-my.sharepoint.com/personal/jhonatan_gomez_wiga_io/Documents/Escritorio/UCO/DOO GIT/SpaOnline/EventStorming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="209" documentId="13_ncr:1_{62893FD2-C189-4ED0-931F-1A498DF7C6B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31275A6B-FA2E-4C11-A0D7-93D7965D25F5}"/>
+  <xr:revisionPtr revIDLastSave="213" documentId="13_ncr:1_{62893FD2-C189-4ED0-931F-1A498DF7C6B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6705F0A5-75A8-411C-91CC-EAD94100FC16}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{36012E7C-B3F4-482B-AC16-7CCB81B9AE88}"/>
+    <workbookView minimized="1" xWindow="11475" yWindow="15" windowWidth="7920" windowHeight="10770" activeTab="2" xr2:uid="{36012E7C-B3F4-482B-AC16-7CCB81B9AE88}"/>
   </bookViews>
   <sheets>
     <sheet name="Flujo de eventos en el tiempo" sheetId="61" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="70">
   <si>
     <t>Descripción</t>
   </si>
@@ -240,10 +240,6 @@
     <t>Pol-Inventario-005</t>
   </si>
   <si>
-    <t xml:space="preserve">No debe existir otro pais, a excepcion de que sea el mismo pais que se esta modificando
- </t>
-  </si>
-  <si>
     <t xml:space="preserve">Debe existir el inventario que se esta modificando </t>
   </si>
   <si>
@@ -269,9 +265,6 @@
  </t>
   </si>
   <si>
-    <t xml:space="preserve">Pol-Inventario-008: </t>
-  </si>
-  <si>
     <t xml:space="preserve">Comando que se encarga de Modificar el inventario validando que lo ingresado este correcto  </t>
   </si>
   <si>
@@ -288,6 +281,17 @@
   </si>
   <si>
     <t>Crear inventario</t>
+  </si>
+  <si>
+    <t>Pol-Inventario-008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No debe existir otro inventario, a excepcion de que sea el mismo inventario que se esta modificando
+ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los datos del nuevo inventario deben ser valido a nivel de tipo de dato, longitud, obligatoriedad, formato, rango
+ </t>
   </si>
 </sst>
 </file>
@@ -776,14 +780,74 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -791,68 +855,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1351,10 +1355,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{235BA608-57CC-45B0-8234-10CA49C3B004}">
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:C9"/>
+    <sheetView tabSelected="1" topLeftCell="F3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1381,84 +1385,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="58" t="str">
+      <c r="B2" s="48" t="str">
         <f>'Listado Objetos de Dominio'!$A$4</f>
         <v>Inventario</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="59"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="49"/>
       <c r="N2" s="4"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="60" t="str">
+      <c r="B3" s="50" t="str">
         <f>'Listado Objetos de Dominio'!$B$4</f>
         <v>Objeto de dominio que contiene la informacion del inventario, según el producto y sucursal</v>
       </c>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
-      <c r="M3" s="61"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="50"/>
+      <c r="M3" s="51"/>
       <c r="N3" s="5"/>
     </row>
     <row r="4" spans="1:14" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="50"/>
+      <c r="C4" s="40"/>
       <c r="D4" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="45" t="s">
+      <c r="E4" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="45"/>
-      <c r="G4" s="53" t="s">
+      <c r="F4" s="52"/>
+      <c r="G4" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="53"/>
+      <c r="H4" s="43"/>
       <c r="I4" s="10" t="s">
         <v>14</v>
       </c>
@@ -1468,52 +1472,52 @@
       <c r="K4" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="56" t="s">
+      <c r="L4" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="57" t="s">
+      <c r="M4" s="47" t="s">
         <v>18</v>
       </c>
       <c r="N4" s="5"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="50" t="s">
+      <c r="C5" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="46" t="s">
+      <c r="D5" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="45" t="s">
+      <c r="E5" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="45"/>
-      <c r="G5" s="51" t="s">
+      <c r="F5" s="52"/>
+      <c r="G5" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="51"/>
-      <c r="I5" s="54" t="s">
+      <c r="H5" s="41"/>
+      <c r="I5" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="55" t="s">
+      <c r="J5" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="52" t="s">
+      <c r="K5" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="56"/>
-      <c r="M5" s="57"/>
+      <c r="L5" s="46"/>
+      <c r="M5" s="47"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="49"/>
-      <c r="B6" s="50"/>
-      <c r="C6" s="50"/>
-      <c r="D6" s="47"/>
+      <c r="A6" s="39"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="37"/>
       <c r="E6" s="18" t="s">
         <v>21</v>
       </c>
@@ -1526,38 +1530,38 @@
       <c r="H6" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="54"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="52"/>
-      <c r="L6" s="56"/>
-      <c r="M6" s="57"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="45"/>
+      <c r="K6" s="42"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="47"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="41" t="s">
+      <c r="C7" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="36" t="s">
+      <c r="D7" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
       <c r="G7" s="13" t="s">
         <v>39</v>
       </c>
       <c r="H7" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="I7" s="36"/>
-      <c r="J7" s="36" t="s">
+      <c r="I7" s="53"/>
+      <c r="J7" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="K7" s="36"/>
+      <c r="K7" s="53"/>
       <c r="L7" s="29" t="s">
         <v>46</v>
       </c>
@@ -1569,21 +1573,21 @@
       <c r="A8" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="37"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="55"/>
       <c r="G8" s="13" t="s">
         <v>41</v>
       </c>
       <c r="H8" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="I8" s="37"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="37"/>
-      <c r="L8" s="36" t="s">
+      <c r="I8" s="55"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="55"/>
+      <c r="L8" s="53" t="s">
         <v>47</v>
       </c>
       <c r="M8" s="30" t="s">
@@ -1594,21 +1598,21 @@
       <c r="A9" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="43"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
+      <c r="B9" s="54"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
       <c r="G9" s="13" t="s">
         <v>43</v>
       </c>
       <c r="H9" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="I9" s="38"/>
-      <c r="J9" s="38"/>
-      <c r="K9" s="38"/>
-      <c r="L9" s="38"/>
+      <c r="I9" s="54"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="54"/>
+      <c r="L9" s="54"/>
       <c r="M9" s="30" t="s">
         <v>50</v>
       </c>
@@ -1617,28 +1621,28 @@
       <c r="A10" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="D10" s="36" t="s">
+      <c r="C10" s="56" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="53"/>
       <c r="G10" s="13" t="s">
         <v>52</v>
       </c>
       <c r="H10" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="I10" s="36"/>
-      <c r="J10" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="K10" s="36"/>
+        <v>68</v>
+      </c>
+      <c r="I10" s="53"/>
+      <c r="J10" s="53" t="s">
+        <v>55</v>
+      </c>
+      <c r="K10" s="53"/>
       <c r="L10" s="29" t="s">
         <v>45</v>
       </c>
@@ -1650,24 +1654,24 @@
       <c r="A11" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="37"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="55"/>
       <c r="G11" s="13" t="s">
         <v>41</v>
       </c>
       <c r="H11" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="I11" s="37"/>
-      <c r="J11" s="37"/>
-      <c r="K11" s="37"/>
-      <c r="L11" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11" s="55"/>
+      <c r="J11" s="55"/>
+      <c r="K11" s="55"/>
+      <c r="L11" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="M11" s="39" t="s">
+      <c r="M11" s="59" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1675,53 +1679,53 @@
       <c r="A12" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="38"/>
-      <c r="C12" s="43"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
+      <c r="B12" s="54"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="54"/>
       <c r="G12" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="I12" s="37"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="38"/>
-      <c r="L12" s="38"/>
-      <c r="M12" s="40"/>
+        <v>53</v>
+      </c>
+      <c r="I12" s="55"/>
+      <c r="J12" s="54"/>
+      <c r="K12" s="54"/>
+      <c r="L12" s="54"/>
+      <c r="M12" s="60"/>
     </row>
     <row r="13" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="53" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="56" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="53" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="53" t="s">
+        <v>59</v>
+      </c>
+      <c r="H13" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="D13" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="H13" s="41" t="s">
-        <v>59</v>
-      </c>
-      <c r="I13" s="36"/>
-      <c r="J13" s="36" t="s">
+      <c r="I13" s="53"/>
+      <c r="J13" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="K13" s="36"/>
+      <c r="K13" s="53"/>
       <c r="L13" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="M13" s="44" t="s">
+      <c r="M13" s="61" t="s">
         <v>50</v>
       </c>
       <c r="N13" s="31"/>
@@ -1730,94 +1734,94 @@
       <c r="A14" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="37"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="37"/>
-      <c r="K14" s="37"/>
+      <c r="B14" s="55"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="54"/>
+      <c r="H14" s="58"/>
+      <c r="I14" s="55"/>
+      <c r="J14" s="55"/>
+      <c r="K14" s="55"/>
       <c r="L14" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="M14" s="44"/>
+      <c r="M14" s="61"/>
     </row>
     <row r="15" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="37"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="36" t="s">
-        <v>62</v>
-      </c>
-      <c r="H15" s="41" t="s">
-        <v>61</v>
-      </c>
-      <c r="I15" s="37"/>
-      <c r="J15" s="37"/>
-      <c r="K15" s="37"/>
-      <c r="L15" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="M15" s="39" t="s">
+      <c r="B15" s="55"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="H15" s="56" t="s">
+        <v>60</v>
+      </c>
+      <c r="I15" s="55"/>
+      <c r="J15" s="55"/>
+      <c r="K15" s="55"/>
+      <c r="L15" s="53" t="s">
+        <v>55</v>
+      </c>
+      <c r="M15" s="59" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B16" s="38"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="43"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="38"/>
-      <c r="K16" s="38"/>
-      <c r="L16" s="38"/>
-      <c r="M16" s="40"/>
+        <v>56</v>
+      </c>
+      <c r="B16" s="54"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="54"/>
+      <c r="H16" s="58"/>
+      <c r="I16" s="54"/>
+      <c r="J16" s="54"/>
+      <c r="K16" s="54"/>
+      <c r="L16" s="54"/>
+      <c r="M16" s="60"/>
     </row>
     <row r="17" spans="1:14" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="41" t="s">
+      <c r="C17" s="56" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="53" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="53"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D17" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="H17" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="I17" s="36"/>
-      <c r="J17" s="36" t="s">
+      <c r="H17" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="I17" s="53"/>
+      <c r="J17" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="K17" s="36"/>
+      <c r="K17" s="53"/>
       <c r="L17" s="29" t="s">
         <v>45</v>
       </c>
       <c r="M17" s="30" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="N17" s="31"/>
     </row>
@@ -1825,20 +1829,20 @@
       <c r="A18" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="37"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="37"/>
-      <c r="K18" s="37"/>
+      <c r="B18" s="55"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="55"/>
+      <c r="F18" s="55"/>
+      <c r="G18" s="55"/>
+      <c r="H18" s="57"/>
+      <c r="I18" s="55"/>
+      <c r="J18" s="55"/>
+      <c r="K18" s="55"/>
       <c r="L18" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="M18" s="39" t="s">
+      <c r="M18" s="59" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1846,98 +1850,69 @@
       <c r="A19" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="38"/>
-      <c r="C19" s="43"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="38"/>
-      <c r="J19" s="38"/>
-      <c r="K19" s="38"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="58"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="54"/>
+      <c r="G19" s="54"/>
+      <c r="H19" s="58"/>
+      <c r="I19" s="54"/>
+      <c r="J19" s="54"/>
+      <c r="K19" s="54"/>
       <c r="L19" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="M19" s="40"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="16"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="16"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="16"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="16"/>
-    </row>
-    <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="14"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="17"/>
+        <v>55</v>
+      </c>
+      <c r="M19" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="62">
+    <mergeCell ref="K17:K19"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="G17:G19"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="I17:I19"/>
+    <mergeCell ref="J17:J19"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="F17:F19"/>
+    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="D13:D16"/>
+    <mergeCell ref="E13:E16"/>
+    <mergeCell ref="F13:F16"/>
+    <mergeCell ref="I13:I16"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="J10:J12"/>
+    <mergeCell ref="K10:K12"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="J13:J16"/>
+    <mergeCell ref="K13:K16"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="J7:J9"/>
+    <mergeCell ref="I7:I9"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="F7:F9"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="A5:A6"/>
@@ -1954,52 +1929,6 @@
     <mergeCell ref="B3:M3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="J7:J9"/>
-    <mergeCell ref="I7:I9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="J10:J12"/>
-    <mergeCell ref="K10:K12"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="J13:J16"/>
-    <mergeCell ref="K13:K16"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="M15:M16"/>
-    <mergeCell ref="I10:I12"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="D13:D16"/>
-    <mergeCell ref="E13:E16"/>
-    <mergeCell ref="F13:F16"/>
-    <mergeCell ref="I13:I16"/>
-    <mergeCell ref="J17:J19"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="E17:E19"/>
-    <mergeCell ref="F17:F19"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="K17:K19"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="G17:G19"/>
-    <mergeCell ref="H17:H19"/>
-    <mergeCell ref="I17:I19"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{F92E8141-0BAA-4CFF-A2AA-790349ADA214}"/>
@@ -2042,84 +1971,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="58" t="str">
+      <c r="B2" s="48" t="str">
         <f>'Listado Objetos de Dominio'!$A$5</f>
         <v>Producto</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="59"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="49"/>
       <c r="N2" s="4"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="60" t="str">
+      <c r="B3" s="50" t="str">
         <f>'Listado Objetos de Dominio'!$B$5</f>
         <v xml:space="preserve">Objeto de dominio que referencia los productos que tiene el inventario </v>
       </c>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
-      <c r="M3" s="61"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="50"/>
+      <c r="M3" s="51"/>
       <c r="N3" s="5"/>
     </row>
     <row r="4" spans="1:14" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="50"/>
+      <c r="C4" s="40"/>
       <c r="D4" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="45" t="s">
+      <c r="E4" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="45"/>
-      <c r="G4" s="53" t="s">
+      <c r="F4" s="52"/>
+      <c r="G4" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="53"/>
+      <c r="H4" s="43"/>
       <c r="I4" s="10" t="s">
         <v>14</v>
       </c>
@@ -2129,52 +2058,52 @@
       <c r="K4" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="56" t="s">
+      <c r="L4" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="57" t="s">
+      <c r="M4" s="47" t="s">
         <v>18</v>
       </c>
       <c r="N4" s="5"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="50" t="s">
+      <c r="C5" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="46" t="s">
+      <c r="D5" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="45" t="s">
+      <c r="E5" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="45"/>
-      <c r="G5" s="51" t="s">
+      <c r="F5" s="52"/>
+      <c r="G5" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="51"/>
-      <c r="I5" s="54" t="s">
+      <c r="H5" s="41"/>
+      <c r="I5" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="55" t="s">
+      <c r="J5" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="52" t="s">
+      <c r="K5" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="56"/>
-      <c r="M5" s="57"/>
+      <c r="L5" s="46"/>
+      <c r="M5" s="47"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="49"/>
-      <c r="B6" s="50"/>
-      <c r="C6" s="50"/>
-      <c r="D6" s="47"/>
+      <c r="A6" s="39"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="37"/>
       <c r="E6" s="18" t="s">
         <v>21</v>
       </c>
@@ -2187,11 +2116,11 @@
       <c r="H6" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="54"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="52"/>
-      <c r="L6" s="56"/>
-      <c r="M6" s="57"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="45"/>
+      <c r="K6" s="42"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="47"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
@@ -2270,6 +2199,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="J5:J6"/>
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="B2:M2"/>
     <mergeCell ref="B3:M3"/>
@@ -2286,7 +2216,6 @@
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{9DF923ED-1686-4B14-A06E-2CBA5434B074}"/>
@@ -2298,21 +2227,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101009649131083C14B4DA86A8CCE286EB917" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="33d994151d56ba12daba8e54dbe95711">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2e7b8f57-5761-4b68-bc8b-a5313b5a9473" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4b2c88e9cfcedcae53c44b46a6fb09bd" ns2:_="">
     <xsd:import namespace="2e7b8f57-5761-4b68-bc8b-a5313b5a9473"/>
@@ -2456,32 +2370,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2038022-656B-4A1B-A485-51A1972238BD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="ff57c5a0-3efd-4333-8513-2b909ca014ae"/>
-    <ds:schemaRef ds:uri="0d2457a1-fe8a-4cb2-a5c3-c59e87d2493e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6724C681-8A04-4D66-BB1C-57F7466573C0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A52D198E-1C75-45AD-8A7E-B98F5C4409CF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2499,6 +2403,31 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6724C681-8A04-4D66-BB1C-57F7466573C0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2038022-656B-4A1B-A485-51A1972238BD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ff57c5a0-3efd-4333-8513-2b909ca014ae"/>
+    <ds:schemaRef ds:uri="0d2457a1-fe8a-4cb2-a5c3-c59e87d2493e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{86cab09b-e61a-4c01-96e7-67fc9e3d8cd5}" enabled="1" method="Standard" siteId="{bf1ce8b5-5d39-4bc5-ad6e-07b3e4d7d67a}" contentBits="8" removed="0"/>

</xml_diff>